<commit_message>
test case for login page
</commit_message>
<xml_diff>
--- a/AssessmentQuestion1/Assessment Question 1 -TestLoginPage.xlsx
+++ b/AssessmentQuestion1/Assessment Question 1 -TestLoginPage.xlsx
@@ -104,9 +104,6 @@
     <t>VALID EMAIL ID AND VALID PASSWORD</t>
   </si>
   <si>
-    <t>INPUT</t>
-  </si>
-  <si>
     <t>com.shipt.ui.loginPage.(story id).005</t>
   </si>
   <si>
@@ -210,6 +207,9 @@
   </si>
   <si>
     <t>Enter a valid email id and valid password associated with the same account. Using key press event in (java.awt) robot class or usign any tool (like selenium - KEYS event), send ENTER key to verify enter key is also working as login button click</t>
+  </si>
+  <si>
+    <t>RE RENTER PASSWORD</t>
   </si>
 </sst>
 </file>
@@ -540,23 +540,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="211.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="218.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="49.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.140625" customWidth="1"/>
+    <col min="7" max="7" width="21.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="52.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="68.140625" customWidth="1"/>
+    <col min="9" max="9" width="69.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -579,13 +579,13 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>26</v>
+        <v>61</v>
       </c>
       <c r="H1" t="s">
         <v>13</v>
       </c>
       <c r="I1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J1" t="s">
         <v>6</v>
@@ -599,10 +599,10 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D2" t="s">
         <v>25</v>
@@ -617,7 +617,7 @@
         <v>14</v>
       </c>
       <c r="I2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J2" t="s">
         <v>8</v>
@@ -634,7 +634,7 @@
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D3" t="s">
         <v>20</v>
@@ -663,19 +663,19 @@
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D4" t="s">
         <v>20</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F4" t="s">
         <v>11</v>
       </c>
       <c r="I4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J4" t="s">
         <v>8</v>
@@ -692,7 +692,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D5" t="s">
         <v>21</v>
@@ -715,13 +715,13 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D6" t="s">
         <v>25</v>
@@ -750,20 +750,20 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E7" s="1"/>
       <c r="H7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J7" t="s">
         <v>8</v>
@@ -774,20 +774,20 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E8" s="1"/>
       <c r="H8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J8" t="s">
         <v>8</v>
@@ -798,23 +798,23 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E9" s="1"/>
       <c r="H9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J9" t="s">
         <v>8</v>
@@ -825,23 +825,23 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E10" s="1"/>
       <c r="H10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J10" t="s">
         <v>8</v>
@@ -852,23 +852,23 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E11" s="1"/>
       <c r="H11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J11" t="s">
         <v>8</v>
@@ -879,23 +879,23 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B12" t="s">
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E12" s="1"/>
       <c r="H12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J12" t="s">
         <v>8</v>
@@ -906,13 +906,13 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D13" t="s">
         <v>25</v>
@@ -927,7 +927,7 @@
         <v>14</v>
       </c>
       <c r="I13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J13" t="s">
         <v>8</v>

</xml_diff>